<commit_message>
feat: added the function to search for linked brands
</commit_message>
<xml_diff>
--- a/relatorio_registros_errados.xlsx
+++ b/relatorio_registros_errados.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="76">
   <si>
     <t>Item</t>
   </si>
@@ -629,8 +629,8 @@
       <c r="C2" t="s">
         <v>54</v>
       </c>
-      <c r="D2" t="s">
-        <v>75</v>
+      <c r="D2">
+        <v>105830220</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -783,8 +783,8 @@
       <c r="C13" t="s">
         <v>61</v>
       </c>
-      <c r="D13" t="s">
-        <v>75</v>
+      <c r="D13">
+        <v>102350779</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -853,8 +853,8 @@
       <c r="C18" t="s">
         <v>63</v>
       </c>
-      <c r="D18" t="s">
-        <v>75</v>
+      <c r="D18">
+        <v>167730219</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1021,8 +1021,8 @@
       <c r="C30" t="s">
         <v>57</v>
       </c>
-      <c r="D30" t="s">
-        <v>75</v>
+      <c r="D30">
+        <v>112360011</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1035,8 +1035,8 @@
       <c r="C31" t="s">
         <v>57</v>
       </c>
-      <c r="D31" t="s">
-        <v>75</v>
+      <c r="D31">
+        <v>112360011</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1203,8 +1203,8 @@
       <c r="C43" t="s">
         <v>70</v>
       </c>
-      <c r="D43" t="s">
-        <v>75</v>
+      <c r="D43">
+        <v>118190327</v>
       </c>
     </row>
     <row r="44" spans="1:4">

</xml_diff>

<commit_message>
refactor: Removing Expired Medications from the DataFrame
</commit_message>
<xml_diff>
--- a/relatorio_registros_errados.xlsx
+++ b/relatorio_registros_errados.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="71">
   <si>
     <t>Item</t>
   </si>
@@ -28,9 +28,6 @@
     <t>Registro</t>
   </si>
   <si>
-    <t>ACETATO DE MEDROXIPROGESTERONA SUSPENSAO INJETAVEL 150 MG/ML</t>
-  </si>
-  <si>
     <t>VALPROATO DE SÓDIO ÁCIDO VALPRÓICO</t>
   </si>
   <si>
@@ -70,9 +67,6 @@
     <t>DEXCLORFENIRAMINA MALEATO 2MG</t>
   </si>
   <si>
-    <t>DIAZEPAM 5 MG</t>
-  </si>
-  <si>
     <t>DINITRATO DE ISOSSORBIDA 5MG SUBLINGUAL</t>
   </si>
   <si>
@@ -106,12 +100,6 @@
     <t>GLICOSIMETROS (MEDIDOR DE GLICOSE)</t>
   </si>
   <si>
-    <t>HALOPERIDOL 1MG</t>
-  </si>
-  <si>
-    <t>HALOPERIDOL 5 MG COMPRIMIDO</t>
-  </si>
-  <si>
     <t>HIDROCORTISONA ACETATO 10MG/G CREME DERMATOLOGICO</t>
   </si>
   <si>
@@ -178,18 +166,18 @@
     <t xml:space="preserve">FITA PARA TESTES DE GLICEMIA COMPATIVEL PARA O APARELHO ACCU-CHEK ACTIVE </t>
   </si>
   <si>
+    <t>BIOLAB SANUS FARMACÊUTICA LTDA</t>
+  </si>
+  <si>
+    <t>GEOLAB INDÚSTRIA FARMACÊUTICA S/A</t>
+  </si>
+  <si>
+    <t>CELLERA FARMACÊUTICA S.A.</t>
+  </si>
+  <si>
     <t>EMS S/A</t>
   </si>
   <si>
-    <t>BIOLAB SANUS FARMACÊUTICA LTDA</t>
-  </si>
-  <si>
-    <t>GEOLAB INDÚSTRIA FARMACÊUTICA S/A</t>
-  </si>
-  <si>
-    <t>CELLERA FARMACÊUTICA S.A.</t>
-  </si>
-  <si>
     <t>BRAINFARMA INDÚSTRIA QUÍMICA E FARMACÊUTICA S.A</t>
   </si>
   <si>
@@ -203,9 +191,6 @@
   </si>
   <si>
     <t>CHIESI FARMACÊUTICA LTDA</t>
-  </si>
-  <si>
-    <t>GERMED FARMACEUTICA LTDA</t>
   </si>
   <si>
     <t>EUROFARMA LABORATÓRIOS S.A.</t>
@@ -599,7 +584,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -621,91 +606,91 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2">
-        <v>105830220</v>
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4" t="s">
-        <v>75</v>
+        <v>51</v>
+      </c>
+      <c r="D4">
+        <v>154230044</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5">
-        <v>154230044</v>
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -714,88 +699,88 @@
         <v>54</v>
       </c>
       <c r="D8" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D10" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" t="s">
-        <v>75</v>
+        <v>54</v>
+      </c>
+      <c r="D11">
+        <v>155840056</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D12">
-        <v>155840056</v>
+        <v>102350779</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D13">
-        <v>102350779</v>
+        <v>100580104</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D14">
         <v>100580104</v>
@@ -803,77 +788,77 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15">
-        <v>100580104</v>
+        <v>51</v>
+      </c>
+      <c r="D15" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D16" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D18">
-        <v>167730219</v>
+        <v>103920213</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D19" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
@@ -881,195 +866,195 @@
       <c r="C20" t="s">
         <v>59</v>
       </c>
-      <c r="D20">
-        <v>103920213</v>
+      <c r="D20" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D21" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B22" t="s">
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D22" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s">
         <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D23" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B24" t="s">
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D24" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="B25" t="s">
         <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D25" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="B26" t="s">
         <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" t="s">
-        <v>75</v>
+        <v>62</v>
+      </c>
+      <c r="D26">
+        <v>105730560</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B27" t="s">
         <v>27</v>
       </c>
       <c r="C27" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D27" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="B28" t="s">
         <v>28</v>
       </c>
       <c r="C28" t="s">
-        <v>67</v>
-      </c>
-      <c r="D28">
-        <v>105730560</v>
+        <v>64</v>
+      </c>
+      <c r="D28" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="B29" t="s">
         <v>29</v>
       </c>
       <c r="C29" t="s">
-        <v>68</v>
-      </c>
-      <c r="D29" t="s">
-        <v>75</v>
+        <v>51</v>
+      </c>
+      <c r="D29">
+        <v>154230227</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="B30" t="s">
         <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>57</v>
-      </c>
-      <c r="D30">
-        <v>112360011</v>
+        <v>50</v>
+      </c>
+      <c r="D30" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B31" t="s">
         <v>31</v>
       </c>
       <c r="C31" t="s">
-        <v>57</v>
-      </c>
-      <c r="D31">
-        <v>112360011</v>
+        <v>62</v>
+      </c>
+      <c r="D31" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="B32" t="s">
         <v>32</v>
       </c>
       <c r="C32" t="s">
-        <v>69</v>
-      </c>
-      <c r="D32" t="s">
-        <v>75</v>
+        <v>51</v>
+      </c>
+      <c r="D32">
+        <v>154230049</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="B33" t="s">
         <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>56</v>
-      </c>
-      <c r="D33">
-        <v>154230227</v>
+        <v>51</v>
+      </c>
+      <c r="D33" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="B34" t="s">
         <v>34</v>
@@ -1078,68 +1063,68 @@
         <v>55</v>
       </c>
       <c r="D34" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="B35" t="s">
         <v>35</v>
       </c>
       <c r="C35" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D35" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B36" t="s">
         <v>36</v>
       </c>
       <c r="C36" t="s">
-        <v>56</v>
-      </c>
-      <c r="D36">
-        <v>154230049</v>
+        <v>61</v>
+      </c>
+      <c r="D36" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="B37" t="s">
         <v>37</v>
       </c>
       <c r="C37" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D37" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B38" t="s">
         <v>38</v>
       </c>
       <c r="C38" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D38" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B39" t="s">
         <v>39</v>
@@ -1147,204 +1132,148 @@
       <c r="C39" t="s">
         <v>65</v>
       </c>
-      <c r="D39" t="s">
-        <v>75</v>
+      <c r="D39">
+        <v>118190327</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B40" t="s">
         <v>40</v>
       </c>
       <c r="C40" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D40" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B41" t="s">
         <v>41</v>
       </c>
       <c r="C41" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="D41" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="B42" t="s">
         <v>42</v>
       </c>
       <c r="C42" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="D42" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B43" t="s">
         <v>43</v>
       </c>
       <c r="C43" t="s">
-        <v>70</v>
-      </c>
-      <c r="D43">
-        <v>118190327</v>
+        <v>67</v>
+      </c>
+      <c r="D43" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="B44" t="s">
         <v>44</v>
       </c>
       <c r="C44" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D44" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="B45" t="s">
         <v>45</v>
       </c>
       <c r="C45" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D45" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="B46" t="s">
         <v>46</v>
       </c>
       <c r="C46" t="s">
-        <v>72</v>
-      </c>
-      <c r="D46" t="s">
-        <v>75</v>
+        <v>57</v>
+      </c>
+      <c r="D46">
+        <v>126750311</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="B47" t="s">
         <v>47</v>
       </c>
       <c r="C47" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="D47" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="B48" t="s">
         <v>48</v>
       </c>
       <c r="C48" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D48" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="B49" t="s">
         <v>49</v>
       </c>
       <c r="C49" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D49" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50">
-        <v>128</v>
-      </c>
-      <c r="B50" t="s">
-        <v>50</v>
-      </c>
-      <c r="C50" t="s">
-        <v>61</v>
-      </c>
-      <c r="D50">
-        <v>126750311</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51">
-        <v>131</v>
-      </c>
-      <c r="B51" t="s">
-        <v>51</v>
-      </c>
-      <c r="C51" t="s">
-        <v>54</v>
-      </c>
-      <c r="D51" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52">
-        <v>135</v>
-      </c>
-      <c r="B52" t="s">
-        <v>52</v>
-      </c>
-      <c r="C52" t="s">
-        <v>74</v>
-      </c>
-      <c r="D52" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53">
-        <v>137</v>
-      </c>
-      <c r="B53" t="s">
-        <v>53</v>
-      </c>
-      <c r="C53" t="s">
-        <v>68</v>
-      </c>
-      <c r="D53" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>